<commit_message>
a lot of update
</commit_message>
<xml_diff>
--- a/Historical Data/指数价2007.xlsx
+++ b/Historical Data/指数价2007.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D4356988-1CE5-466D-A305-471D253CFF04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8DF8CCBB-7318-468A-9FA4-A1454F6FF009}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>000016.SH</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,10 @@
   </si>
   <si>
     <t>000036.SH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -383,13 +387,15 @@
   <dimension ref="A1:H2840"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>